<commit_message>
updated Gender xpath to Sex xpath for canine
</commit_message>
<xml_diff>
--- a/OutputFiles/TC01_Canine_Filter_Gender-CastratedMale_Neo4jData.xlsx
+++ b/OutputFiles/TC01_Canine_Filter_Gender-CastratedMale_Neo4jData.xlsx
@@ -8,12 +8,15 @@
   <sheets>
     <sheet name="CypherOutput" r:id="rId3" sheetId="1"/>
     <sheet name="Message" r:id="rId4" sheetId="2"/>
+    <sheet name="CypherOutput_Message" r:id="rId5" sheetId="3"/>
+    <sheet name="StatOutput" r:id="rId6" sheetId="4"/>
+    <sheet name="StatOutput_Message" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="131">
   <si>
     <t>Case ID</t>
   </si>
@@ -400,6 +403,12 @@
   </si>
   <si>
     <t>C:\Users\radhakrishnang2\Desktop\Commons_Automation\OutputFiles\TC01_Canine_Filter_Gender-CastratedMale_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\radhakrishnang2\Desktop\Script\Commons_Automation\OutputFiles\TC01_Canine_Filter_Gender-CastratedMale_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>Cypher query should not be an empty string</t>
   </si>
 </sst>
 </file>
@@ -434,10 +443,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -446,7 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
@@ -1792,4 +1801,199 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1"/>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>